<commit_message>
Modifying excel data format
</commit_message>
<xml_diff>
--- a/Abot.xlsx
+++ b/Abot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapas/workspace/Excel-For-CICD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CEFC9A-38BA-4549-A315-167D034D2083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7DD4FC-FB92-C848-8E59-3D7CFA804505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>WL 5G SA Daily Regression through Magma CICD pipeline</t>
   </si>
@@ -73,10 +73,13 @@
     <t>MGM-5GSA-FUNC-TC005</t>
   </si>
   <si>
-    <t>passed</t>
-  </si>
-  <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Result For</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -95,6 +98,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -449,15 +453,18 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="59.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +506,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -510,7 +517,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>